<commit_message>
urban population by ethnicity
</commit_message>
<xml_diff>
--- a/data/ethnicity_info.xlsx
+++ b/data/ethnicity_info.xlsx
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\Thesis2\Geopolitics of repressions\Geopolitics-of-Repressions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C20EF9-0340-4B79-A548-B95C6EAD3ADB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C11E4B9-BF6F-4EFA-BF82-10581F5473F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6516" yWindow="1896" windowWidth="18432" windowHeight="8772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7536" yWindow="1464" windowWidth="18432" windowHeight="8772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ethnicity</t>
   </si>
@@ -76,17 +84,26 @@
     <t>Ukrainian</t>
   </si>
   <si>
-    <t>population</t>
-  </si>
-  <si>
     <t>clad_sim</t>
+  </si>
+  <si>
+    <t>urb_rate</t>
+  </si>
+  <si>
+    <t>urban_pop</t>
+  </si>
+  <si>
+    <t>pop_total</t>
+  </si>
+  <si>
+    <t>rural_pop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +118,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,18 +151,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Procenta" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,18 +514,27 @@
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -500,8 +544,19 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>555675</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E15" si="0">B2-D2</f>
+        <v>1011893</v>
+      </c>
+      <c r="F2" s="4">
+        <f>D2/B2</f>
+        <v>0.35448222979800559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -511,8 +566,19 @@
       <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>489115</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>4249808</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F18" si="1">D3/B3</f>
+        <v>0.10321226996091729</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -522,8 +588,19 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>35578</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>119088</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.23003116392743073</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -533,8 +610,19 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>184769</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1053780</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.14918182486118836</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -544,8 +632,19 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>45347</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>168418</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.21213482094823755</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -555,8 +654,19 @@
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>3111</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>315411</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7669862678245144E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -566,8 +676,19 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>6647</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>3600</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.64867766175465991</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -577,8 +698,19 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>2143262</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>456711</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="1"/>
+        <v>0.8243400989164118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -588,8 +720,19 @@
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>1781</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>138144</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>1.2728247275326067E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -599,8 +742,19 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>1670</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>127651</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>1.2913602585813595E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -610,8 +764,19 @@
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>9156</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>77843</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.1052425889952758</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -621,8 +786,19 @@
       <c r="C13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>59959</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>81744</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="1"/>
+        <v>0.42313147922062344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -632,8 +808,19 @@
       <c r="C14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>26190</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>15273</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>0.6316474929455177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -643,8 +830,19 @@
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>21392</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>250880</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>7.8568490333196211E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -654,8 +852,19 @@
       <c r="C16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>256185</v>
+      </c>
+      <c r="E16">
+        <f>B16-D16</f>
+        <v>526149</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.3274624393162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -665,8 +874,19 @@
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>451440</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E18" si="2">B17-D17</f>
+        <v>2465096</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="1"/>
+        <v>0.15478636300049101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -675,6 +895,17 @@
       </c>
       <c r="C18">
         <v>4</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3286945</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>27908031</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10536776819446823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>